<commit_message>
add phase 1.1 & 1.2
</commit_message>
<xml_diff>
--- a/Dokumentation/project plan.xlsx
+++ b/Dokumentation/project plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebiru\code\Informatik-2.Jahr\IPT6.1\IPT6.1-Productivity-Game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebiru\code\Informatik-2.Jahr\IPT6.1\IPT6.1-Productivity-Game\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB6BBE7F-E39B-498E-A965-2A31CC95C58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A5269B-80C5-4C4B-BBEF-86DA76A5077C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -52,35 +52,15 @@
     <t>Topic:</t>
   </si>
   <si>
-    <t>Technology</t>
-  </si>
-  <si>
-    <t>Keywords:</t>
-  </si>
-  <si>
-    <t>Innovative, fresh, elegant</t>
-  </si>
-  <si>
     <t>Name:</t>
   </si>
   <si>
-    <t>Team Dev</t>
-  </si>
-  <si>
     <t>Goal:</t>
   </si>
   <si>
     <t>Objective:</t>
   </si>
   <si>
-    <t xml:space="preserve">To win a grant or scholarships and a trip to Silicon Valley and Seattle.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Develop a technology solution for submission to the upcoming innovative app competition.
-</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Task Status Indicator</t>
   </si>
   <si>
@@ -99,31 +79,49 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Review competition rules</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Add links to project resources here</t>
-  </si>
-  <si>
-    <t>Research prior winning technologies</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Develop &amp; test app</t>
-  </si>
-  <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>Write documentation</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Plan Due Date:</t>
+    <t>Egor, Sanjivan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Project Due Date:</t>
+  </si>
+  <si>
+    <t>Productivity-Game</t>
+  </si>
+  <si>
+    <t>Phase 1.1: Projektdefinition</t>
+  </si>
+  <si>
+    <t>Ziel der Anwendung schriftlich festhalten</t>
+  </si>
+  <si>
+    <t>Funktionbeschreibung</t>
+  </si>
+  <si>
+    <t>Tasksverwaltung</t>
+  </si>
+  <si>
+    <t>Phase 1.2: Feature-Liste &amp; Use-Cases</t>
+  </si>
+  <si>
+    <t>Features auflisten (CRUD)</t>
+  </si>
+  <si>
+    <t>Wie wird XP berechnt &amp; gespeichert</t>
+  </si>
+  <si>
+    <t>Level bestimmen</t>
+  </si>
+  <si>
+    <t>Streak aktualisieren</t>
+  </si>
+  <si>
+    <t>Wichtige Use-Cases beschreiben </t>
   </si>
 </sst>
 </file>
@@ -233,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +253,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +351,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -378,6 +382,9 @@
     <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="19" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -390,8 +397,38 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="7">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="19">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="9" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="18" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="5" borderId="0" xfId="19" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="19" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -416,7 +453,47 @@
     <cellStyle name="Task Indicator" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="5" tint="-0.499984740745262"/>
@@ -495,10 +572,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Idea Planner" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Idea Planner" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstColumn" dxfId="4"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
+      <tableStyleElement type="headerRow" dxfId="11"/>
+      <tableStyleElement type="firstColumn" dxfId="10"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -523,9 +600,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>425938</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -568,8 +645,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B6:G10" totalsRowShown="0">
-  <autoFilter ref="B6:G10" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B6:G17" totalsRowShown="0">
+  <autoFilter ref="B6:G17" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -865,10 +942,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G10"/>
+  <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -884,129 +961,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5">
+        <v>46185</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="5">
-        <f ca="1">TODAY()</f>
-        <v>46058</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="2:7" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="8" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="8">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="7">
-        <f ca="1">PlanDueDate-15</f>
-        <v>46043</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="9">
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="21" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
+        <v/>
+      </c>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="8">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" s="7">
-        <f ca="1">PlanDueDate-12</f>
-        <v>46046</v>
+        <f ca="1">TODAY()</f>
+        <v>46058</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F8" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1015,14 +1076,14 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D9" s="7">
-        <f ca="1">PlanDueDate-10</f>
-        <v>46048</v>
+        <f ca="1">TODAY()</f>
+        <v>46058</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F9" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
@@ -1032,21 +1093,144 @@
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="8">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" s="7">
-        <f ca="1">PlanDueDate-5</f>
-        <v>46053</v>
+        <f ca="1">TODAY()</f>
+        <v>46058</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F10" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="15" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G11" s="22"/>
+    </row>
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="15">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="16">
+        <v>46198</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="15">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="15">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="16">
+        <v>46199</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="15">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="15">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="16">
+        <v>46200</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="15">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="16">
+        <v>46201</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="15">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="15">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="16">
+        <v>46202</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="15">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="15" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="15" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1058,7 +1242,7 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B10">
+  <conditionalFormatting sqref="B7:B17">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="-1"/>
@@ -1070,14 +1254,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F10">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="F7:F17">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>F7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>F7=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>F7=-1</formula>
     </cfRule>
     <cfRule type="iconSet" priority="18">
@@ -1088,13 +1272,12 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="198" yWindow="610" count="22">
+  <dataValidations xWindow="1660" yWindow="543" count="21">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Idea Planner in this worksheet. Set a Goal and an Objective, and enter task details in the Tasks table" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Image is in this cell. Title of this worksheet is in cell below" sqref="B1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Topic in cell at right" sqref="D2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Topic in this cell" sqref="E2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Keywords in cell at right" sqref="F2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Keywords in this cell" sqref="G2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Keywords in cell at right" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Plan Due Date in cell at right" sqref="D3" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Plan Due Date in this cell" sqref="E3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Name in cell at right" sqref="F3" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
@@ -1110,7 +1293,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Status icons in this column are automatically updated based on Done column value &amp; comparing Due Dates. Dates beyond the due date &amp; just before the due date are noted for emphasis" sqref="F6" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in this cell" sqref="E5:G5" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter idea details in cells at right. Enter Goal and Objective below. Enter tasks in Tasks table below" sqref="B2:C3" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E10" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E17" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>"Yes, No, Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add phase 2(without dates)
</commit_message>
<xml_diff>
--- a/Dokumentation/project plan.xlsx
+++ b/Dokumentation/project plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebiru\code\Informatik-2.Jahr\IPT6.1\IPT6.1-Productivity-Game\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FA2F80-0229-4BF4-B26D-BCE5B8EF3A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1FB1AE-456D-43B8-8634-BF196386AFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6000" yWindow="-21600" windowWidth="24390" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Idea Planner" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -149,6 +149,75 @@
   </si>
   <si>
     <t>PAP erstellen (PapDesigner)</t>
+  </si>
+  <si>
+    <t>Phase 2.1: Seitenstruktur</t>
+  </si>
+  <si>
+    <t>Seiten festlegen</t>
+  </si>
+  <si>
+    <t>Zwecks- und Funktionsdefinition</t>
+  </si>
+  <si>
+    <t>Navigations bestimmen</t>
+  </si>
+  <si>
+    <t>Benutzerabläufe festlegen</t>
+  </si>
+  <si>
+    <t>Phase 2.2: Wireframes</t>
+  </si>
+  <si>
+    <t>Wireframe-Tool auswählen</t>
+  </si>
+  <si>
+    <t>Wireframes erstellen</t>
+  </si>
+  <si>
+    <t>Wireframes exportieren und ablegen</t>
+  </si>
+  <si>
+    <t>Mockup</t>
+  </si>
+  <si>
+    <t>Farben, Typographie und Abstände definieren</t>
+  </si>
+  <si>
+    <t>UI-Komponenten ausarbeiten</t>
+  </si>
+  <si>
+    <t>Einheitliches Design festlegen</t>
+  </si>
+  <si>
+    <t>Mockup exportieren und ablegen</t>
+  </si>
+  <si>
+    <t>Entitäten festlegen</t>
+  </si>
+  <si>
+    <t>attribute, datentypen, PK festlegen</t>
+  </si>
+  <si>
+    <t>Beziehungen definieren</t>
+  </si>
+  <si>
+    <t>Kardinalitäten bestimmen</t>
+  </si>
+  <si>
+    <t>ER Diagramm erstellen</t>
+  </si>
+  <si>
+    <t>Relationales Diagramm erstellen</t>
+  </si>
+  <si>
+    <t>Diagramme ablegen</t>
+  </si>
+  <si>
+    <t>Phase 2.4: Datenmodell (DB)</t>
+  </si>
+  <si>
+    <t>Phase 2.3: Mockup-Erstellung</t>
   </si>
 </sst>
 </file>
@@ -384,7 +453,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -451,6 +520,33 @@
     <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="19" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="18" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="6" borderId="0" xfId="19" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -463,35 +559,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="7">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="18" applyFont="1" applyFill="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="18" applyFont="1" applyFill="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="9" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="9" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="6" borderId="0" xfId="19" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="19" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="168" fontId="12" fillId="4" borderId="0" xfId="19" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -516,7 +588,67 @@
     <cellStyle name="Task Indicator" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="5" tint="-0.499984740745262"/>
@@ -559,26 +691,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="&quot;Complete&quot;;&quot;Incomplete or Overdue&quot;;&quot;Pending or Due Tomorrow&quot;"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -638,10 +750,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Idea Planner" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Idea Planner" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="firstColumn" dxfId="11"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="19"/>
+      <tableStyleElement type="headerRow" dxfId="18"/>
+      <tableStyleElement type="firstColumn" dxfId="17"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="16"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -711,8 +823,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B6:G30" totalsRowShown="0">
-  <autoFilter ref="B6:G30" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B6:G73" totalsRowShown="0">
+  <autoFilter ref="B6:G73" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -730,7 +842,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status Icon" dataCellStyle="Status Icon Text">
       <calculatedColumnFormula>IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Notes" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Notes" dataDxfId="15">
       <calculatedColumnFormula>IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1010,10 +1122,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G30"/>
+  <dimension ref="B1:G73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1029,14 +1141,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1047,8 +1159,8 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="10" t="s">
         <v>14</v>
       </c>
@@ -1063,24 +1175,24 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="2:7" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
@@ -1116,7 +1228,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
       </c>
-      <c r="G7" s="30" t="str">
+      <c r="G7" s="26" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
       </c>
@@ -1131,7 +1243,7 @@
       </c>
       <c r="D8" s="7">
         <f ca="1">TODAY()</f>
-        <v>46058</v>
+        <v>46062</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>12</v>
@@ -1140,7 +1252,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>0</v>
       </c>
-      <c r="G8" s="31"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="8">
@@ -1152,7 +1264,7 @@
       </c>
       <c r="D9" s="7">
         <f ca="1">TODAY()</f>
-        <v>46058</v>
+        <v>46062</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>12</v>
@@ -1161,7 +1273,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>0</v>
       </c>
-      <c r="G9" s="31"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="8">
@@ -1173,7 +1285,7 @@
       </c>
       <c r="D10" s="7">
         <f ca="1">TODAY()</f>
-        <v>46058</v>
+        <v>46062</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>12</v>
@@ -1182,7 +1294,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>0</v>
       </c>
-      <c r="G10" s="31"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="11" t="str">
@@ -1198,7 +1310,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
       </c>
-      <c r="G11" s="32"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
@@ -1218,7 +1330,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G12" s="31"/>
+      <c r="G12" s="27"/>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="11">
@@ -1238,7 +1350,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="27"/>
     </row>
     <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11">
@@ -1258,7 +1370,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11">
@@ -1278,7 +1390,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G15" s="31"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
@@ -1298,23 +1410,23 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G16" s="31"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G17" s="33"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G17" s="29"/>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
@@ -1374,23 +1486,23 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G20" s="34"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G21" s="29"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G21" s="25"/>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="11">
@@ -1410,7 +1522,7 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G22" s="35"/>
+      <c r="G22" s="30"/>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="11">
@@ -1437,16 +1549,16 @@
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="29" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G24" s="29"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="11">
@@ -1473,18 +1585,24 @@
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G26" s="11"/>
+      <c r="C26" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="35"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="17" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
@@ -1499,6 +1617,9 @@
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
       <c r="D28" s="12"/>
       <c r="E28" s="13"/>
       <c r="F28" s="11" t="str">
@@ -1512,6 +1633,9 @@
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
       <c r="F29" s="11" t="str">
@@ -1525,6 +1649,9 @@
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
       <c r="D30" s="12"/>
       <c r="E30" s="13"/>
       <c r="F30" s="11" t="str">
@@ -1532,6 +1659,622 @@
         <v/>
       </c>
       <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="35"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="17" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G31" s="26"/>
+    </row>
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G32" s="27"/>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G33" s="27"/>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G34" s="27"/>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="35"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="17" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G35" s="26"/>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G36" s="27"/>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G37" s="27"/>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G38" s="27"/>
+    </row>
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G39" s="27"/>
+    </row>
+    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G40" s="27"/>
+    </row>
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="17" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G41" s="26"/>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G42" s="27"/>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G43" s="27"/>
+    </row>
+    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C44" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G44" s="27" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G45" s="27"/>
+    </row>
+    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G46" s="27"/>
+    </row>
+    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G47" s="27"/>
+    </row>
+    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G48" s="27"/>
+    </row>
+    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G49" s="27"/>
+    </row>
+    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G50" s="27"/>
+    </row>
+    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D51" s="12"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G51" s="27"/>
+    </row>
+    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D52" s="12"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G52" s="27"/>
+    </row>
+    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G53" s="27"/>
+    </row>
+    <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D54" s="12"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G54" s="27"/>
+    </row>
+    <row r="55" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G55" s="27"/>
+    </row>
+    <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G56" s="27"/>
+    </row>
+    <row r="57" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D57" s="12"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G57" s="27"/>
+    </row>
+    <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G58" s="27"/>
+    </row>
+    <row r="59" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D59" s="12"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G59" s="27"/>
+    </row>
+    <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D60" s="12"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G60" s="27"/>
+    </row>
+    <row r="61" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G61" s="27"/>
+    </row>
+    <row r="62" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G62" s="27"/>
+    </row>
+    <row r="63" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G63" s="27"/>
+    </row>
+    <row r="64" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D64" s="12"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G64" s="27"/>
+    </row>
+    <row r="65" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D65" s="12"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G65" s="27"/>
+    </row>
+    <row r="66" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D66" s="12"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G66" s="27"/>
+    </row>
+    <row r="67" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D67" s="12"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G67" s="27"/>
+    </row>
+    <row r="68" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B68" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D68" s="12"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G68" s="27"/>
+    </row>
+    <row r="69" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D69" s="12"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G69" s="27"/>
+    </row>
+    <row r="70" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D70" s="12"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G70" s="27"/>
+    </row>
+    <row r="71" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B71" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D71" s="12"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G71" s="27"/>
+    </row>
+    <row r="72" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D72" s="12"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G72" s="27"/>
+    </row>
+    <row r="73" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D73" s="12"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G73" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1542,7 +2285,7 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B30">
+  <conditionalFormatting sqref="B7:B73">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="-1"/>
@@ -1554,14 +2297,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F30">
-    <cfRule type="expression" dxfId="5" priority="5">
+  <conditionalFormatting sqref="F7:F73">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>F7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>F7=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>F7=-1</formula>
     </cfRule>
     <cfRule type="iconSet" priority="22">
@@ -1573,13 +2316,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G30">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>G18=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>G18=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>G18=-1</formula>
     </cfRule>
     <cfRule type="iconSet" priority="4">
@@ -1611,7 +2354,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Status icons in this column are automatically updated based on Done column value &amp; comparing Due Dates. Dates beyond the due date &amp; just before the due date are noted for emphasis" sqref="F6" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in this cell" sqref="E5:G5" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter idea details in cells at right. Enter Goal and Objective below. Enter tasks in Tasks table below" sqref="B2:C3" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E30" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E73" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>"Yes, No, Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>